<commit_message>
Backups of Code and Data
Because I’m experimenting w/ my computer, I’m going to back up all my
data right now.
</commit_message>
<xml_diff>
--- a/Verified_Data/Stat_Argument.xlsx
+++ b/Verified_Data/Stat_Argument.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="0" windowWidth="19540" windowHeight="19040" tabRatio="500" activeTab="5"/>
+    <workbookView minimized="1" xWindow="3660" yWindow="460" windowWidth="25600" windowHeight="16980" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IC 2391" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="112">
   <si>
     <t>J-Count</t>
   </si>
@@ -354,6 +354,12 @@
   </si>
   <si>
     <t>Abs Mag</t>
+  </si>
+  <si>
+    <t>Below 4.5 DelK</t>
+  </si>
+  <si>
+    <t>HD73722</t>
   </si>
 </sst>
 </file>
@@ -366,7 +372,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -405,8 +411,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,8 +442,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -429,7 +471,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="285">
+  <cellStyleXfs count="336">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -715,8 +757,59 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,20 +835,46 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="7" fillId="4" borderId="0" xfId="287" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="0" xfId="286" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="4" borderId="0" xfId="287" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="0" xfId="286" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="285" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="285" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="285">
+  <cellStyles count="336">
+    <cellStyle name="Bad" xfId="286" builtinId="27"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -898,6 +1017,31 @@
     <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Good" xfId="285" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1040,6 +1184,31 @@
     <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="287" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1369,10 +1538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1384,10 +1553,12 @@
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
     <col min="6" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="4.1640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="17.33203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1418,8 +1589,11 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1454,8 +1628,12 @@
       <c r="L2" s="7">
         <v>0.99967185163600003</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -1487,8 +1665,12 @@
       <c r="L3" s="7">
         <v>0.99826639072300005</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -1512,19 +1694,23 @@
         <v>-2.8068400111748719</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="J4" s="7">
-        <v>0.99916441709100001</v>
+        <v>0.99987678713499994</v>
       </c>
       <c r="K4" s="7">
-        <v>0.99852071424900002</v>
+        <v>0.99974472134699999</v>
       </c>
       <c r="L4" s="7">
-        <v>0.99826639072300005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>0.99967185163600003</v>
+      </c>
+      <c r="M4" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -1548,19 +1734,23 @@
         <v>-2.3068400111748719</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J5" s="7">
-        <v>0.99968264681300001</v>
+        <v>0.99692807331199995</v>
       </c>
       <c r="K5" s="7">
-        <v>0.99936385265399996</v>
+        <v>0.99778949223199997</v>
       </c>
       <c r="L5" s="7">
-        <v>0.99949239888700003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
+        <v>0.99743437210899999</v>
+      </c>
+      <c r="M5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1581,19 +1771,23 @@
         <v>-1.8068400111748719</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="7">
-        <v>0.99995564933299996</v>
+        <v>0.99968264681300001</v>
       </c>
       <c r="K6" s="7">
-        <v>0.99990397364500005</v>
+        <v>0.99936385265399996</v>
       </c>
       <c r="L6" s="7">
-        <v>0.99986907478499998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>0.99949239888700003</v>
+      </c>
+      <c r="M6" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1617,19 +1811,23 @@
         <v>-1.3068400111748719</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="9">
-        <v>0.98976183763100001</v>
+        <v>44</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.99995564933299996</v>
       </c>
       <c r="K7" s="7">
-        <v>0.99507985451699998</v>
+        <v>0.99990397364500005</v>
       </c>
       <c r="L7" s="7">
-        <v>0.99619263880499997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>0.99986907478499998</v>
+      </c>
+      <c r="M7" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1652,8 +1850,24 @@
         <f>F8-(5*LOG(E8, 10)-5)</f>
         <v>-0.80684001117487192</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="I8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.99308127647400002</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.99507985451699998</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.99440656781299996</v>
+      </c>
+      <c r="M8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -1673,8 +1887,9 @@
         <f>F9-(5*LOG(E8, 10)-5)</f>
         <v>-0.30684001117487192</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -1694,8 +1909,9 @@
         <f>F10-(5*LOG(E8, 10)-5)</f>
         <v>0.19315998882512808</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10"/>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -1715,8 +1931,9 @@
         <f>F11-(5*LOG(E8, 10)-5)</f>
         <v>0.69315998882512808</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -1736,8 +1953,9 @@
         <f>F12-(5*LOG(E8, 10)-5)</f>
         <v>1.1931599888251281</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1757,8 +1975,9 @@
         <f>F13-(5*LOG(E8, 10)-5)</f>
         <v>1.6931599888251281</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1778,8 +1997,9 @@
         <f>F14-(5*LOG(E8, 10)-5)</f>
         <v>2.1931599888251281</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1799,8 +2019,9 @@
         <f>F15-(5*LOG(E8, 10)-5)</f>
         <v>2.6931599888251281</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -1820,8 +2041,9 @@
         <f>F16-(5*LOG(E8, 10)-5)</f>
         <v>3.1931599888251281</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1841,8 +2063,9 @@
         <f>F17-(5*LOG(E8, 10)-5)</f>
         <v>3.6931599888251281</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -1862,8 +2085,9 @@
         <f>F18-(5*LOG(E8, 10)-5)</f>
         <v>4.1931599888251281</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1883,8 +2107,9 @@
         <f>F19-(5*LOG(E8, 10)-5)</f>
         <v>4.6931599888251281</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1904,8 +2129,9 @@
         <f>F20-(5*LOG(E8, 10)-5)</f>
         <v>5.1931599888251281</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1926,7 +2152,7 @@
         <v>5.6931599888251281</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1947,7 +2173,7 @@
         <v>6.1931599888251281</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1968,7 +2194,7 @@
         <v>6.6931599888251281</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1989,7 +2215,7 @@
         <v>7.1931599888251281</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -2010,7 +2236,7 @@
         <v>7.6931599888251281</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -2031,7 +2257,7 @@
         <v>8.1931599888251281</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -2052,7 +2278,7 @@
         <v>8.6931599888251281</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -2073,7 +2299,7 @@
         <v>9.1931599888251281</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:13">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -2090,7 +2316,7 @@
         <v>405874</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:13">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -2110,8 +2336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2124,7 +2350,9 @@
     <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="1"/>
     <col min="8" max="8" width="5.33203125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="9" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="14.5" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -2161,6 +2389,9 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
@@ -2188,14 +2419,18 @@
       <c r="I2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="13">
         <v>0.94722860581500001</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="14">
         <v>0.89497240252599997</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="14">
         <v>0.87363996218899997</v>
+      </c>
+      <c r="M2" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -2230,6 +2465,10 @@
       <c r="L3" s="7">
         <v>0.99979798623899996</v>
       </c>
+      <c r="M3" s="9" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
@@ -2257,14 +2496,18 @@
       <c r="I4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="14">
         <v>0.88399385936899999</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="14">
         <v>0.89497240252599997</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="14">
         <v>0.87363996218899997</v>
+      </c>
+      <c r="M4" s="16" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2302,6 +2545,10 @@
       <c r="L5" s="7">
         <v>0.99918632300599997</v>
       </c>
+      <c r="M5" s="9" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
@@ -2326,18 +2573,18 @@
       <c r="I6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="14">
         <v>0.83260482399500002</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="14">
         <v>0.791184737237</v>
       </c>
-      <c r="L6" s="9">
+      <c r="L6" s="14">
         <v>0.75233804358400003</v>
       </c>
-      <c r="M6" s="1">
-        <f>L6^20</f>
-        <v>3.3748965738036253E-3</v>
+      <c r="M6" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2363,6 +2610,7 @@
         <f>F7-(5*LOG(E8, 10)-5)</f>
         <v>-2.6568188207949373</v>
       </c>
+      <c r="M7" s="9"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
@@ -2387,6 +2635,7 @@
         <f>F8-(5*LOG(E8, 10)-5)</f>
         <v>-2.1568188207949373</v>
       </c>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
@@ -2408,6 +2657,7 @@
         <f>F9-(5*LOG(E8, 10)-5)</f>
         <v>-1.6568188207949373</v>
       </c>
+      <c r="M9" s="9"/>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
@@ -2429,6 +2679,7 @@
         <f>F10-(5*LOG(E8, 10)-5)</f>
         <v>-1.1568188207949373</v>
       </c>
+      <c r="M10" s="9"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
@@ -2450,6 +2701,7 @@
         <f>F11-(5*LOG(E8, 10)-5)</f>
         <v>-0.65681882079493725</v>
       </c>
+      <c r="M11" s="9"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
@@ -3105,10 +3357,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3118,10 +3370,12 @@
     <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="14.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -3152,8 +3406,11 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3188,8 +3445,12 @@
       <c r="L2" s="8">
         <v>0.95735788444600001</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3221,8 +3482,12 @@
       <c r="L3" s="8">
         <v>0.99959409415199996</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -3257,8 +3522,12 @@
       <c r="L4" s="8">
         <v>0.98599045987599998</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -3284,7 +3553,7 @@
       <c r="I5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5" s="11">
         <v>0.946062598373</v>
       </c>
       <c r="K5" s="8">
@@ -3293,8 +3562,12 @@
       <c r="L5" s="8">
         <v>0.95735788444600001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3326,8 +3599,12 @@
       <c r="L6" s="8">
         <v>0.99972248895000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -3362,8 +3639,12 @@
       <c r="L7" s="8">
         <v>0.98599045987599998</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -3398,8 +3679,12 @@
       <c r="L8" s="8">
         <v>0.97001931921899998</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -3431,8 +3716,12 @@
       <c r="L9" s="8">
         <v>0.99689417686500004</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -3464,8 +3753,12 @@
       <c r="L10" s="8">
         <v>0.99904682273000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -3497,8 +3790,12 @@
       <c r="L11" s="8">
         <v>0.99544287808200005</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -3530,8 +3827,12 @@
       <c r="L12" s="8">
         <v>0.99959409415199996</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -3554,17 +3855,21 @@
       <c r="I13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J13" s="10">
+      <c r="J13" s="11">
         <v>0.92478586480799996</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="11">
         <v>0.94582249225799997</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="11">
         <v>0.93869179196899999</v>
       </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3596,8 +3901,12 @@
       <c r="L14" s="8">
         <v>0.99938409072000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -3617,8 +3926,9 @@
         <f>F15-(5*LOG(E8, 10)-5)</f>
         <v>2.1759108849523177</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="18"/>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -3638,8 +3948,9 @@
         <f>F16-(5*LOG(E8, 10)-5)</f>
         <v>2.6759108849523177</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -3659,8 +3970,9 @@
         <f>F17-(5*LOG(E8, 10)-5)</f>
         <v>3.1759108849523177</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -3680,8 +3992,9 @@
         <f>F18-(5*LOG(E8, 10)-5)</f>
         <v>3.6759108849523177</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -3701,8 +4014,9 @@
         <f>F19-(5*LOG(E8, 10)-5)</f>
         <v>4.1759108849523177</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -3722,8 +4036,9 @@
         <f>F20-(5*LOG(E8, 10)-5)</f>
         <v>4.6759108849523177</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -3743,8 +4058,9 @@
         <f>F21-(5*LOG(E8, 10)-5)</f>
         <v>5.1759108849523177</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -3764,8 +4080,9 @@
         <f>F22-(5*LOG(E8, 10)-5)</f>
         <v>5.6759108849523177</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -3785,8 +4102,9 @@
         <f>F23-(5*LOG(E8, 10)-5)</f>
         <v>6.1759108849523177</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="M23" s="18"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -3806,8 +4124,9 @@
         <f>F24-(5*LOG(E8, 10)-5)</f>
         <v>6.6759108849523177</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -3827,8 +4146,9 @@
         <f>F25-(5*LOG(E8, 10)-5)</f>
         <v>7.1759108849523177</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="M25" s="18"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -3848,8 +4168,9 @@
         <f>F26-(5*LOG(E8, 10)-5)</f>
         <v>7.6759108849523177</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="M26" s="19"/>
+    </row>
+    <row r="27" spans="1:13">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -3869,8 +4190,9 @@
         <f>F27-(5*LOG(E8, 10)-5)</f>
         <v>8.1759108849523177</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="M27" s="20"/>
+    </row>
+    <row r="28" spans="1:13">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -3890,8 +4212,9 @@
         <f>F28-(5*LOG(E8, 10)-5)</f>
         <v>8.6759108849523177</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="M28" s="18"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="1" t="s">
         <v>99</v>
       </c>
@@ -3911,8 +4234,9 @@
         <f>F29-(5*LOG(E8, 10)-5)</f>
         <v>9.1759108849523177</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="M29" s="18"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="1" t="s">
         <v>100</v>
       </c>
@@ -3933,7 +4257,7 @@
         <v>9.6759108849523177</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:13">
       <c r="A31" s="1" t="s">
         <v>101</v>
       </c>
@@ -3954,7 +4278,7 @@
         <v>10.175910884952318</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:13">
       <c r="A32" s="1" t="s">
         <v>102</v>
       </c>
@@ -4054,7 +4378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A29" sqref="A29:A35"/>
     </sheetView>
   </sheetViews>
@@ -4695,7 +5019,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B29" s="1">
@@ -4716,7 +5040,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B30" s="1">
@@ -4737,7 +5061,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="1">
@@ -4758,7 +5082,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="1">
@@ -4779,7 +5103,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B33" s="1">
@@ -4800,7 +5124,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="1">
@@ -4821,7 +5145,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B35" s="1">
@@ -4876,10 +5200,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4889,10 +5213,12 @@
     <col min="3" max="3" width="11.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="15.83203125" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4923,8 +5249,11 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4959,8 +5288,12 @@
       <c r="L2" s="8">
         <v>0.99828274432999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -4986,14 +5319,18 @@
       <c r="J3" s="8">
         <v>0.95257070962699997</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3" s="11">
         <v>0.948539697761</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="11">
         <v>0.94015559416399996</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -5019,17 +5356,21 @@
       <c r="I4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="12">
         <v>0.67203252954000003</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="12">
         <v>0.68463815129299999</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="12">
         <v>0.78123242986300001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -5061,11 +5402,15 @@
       <c r="K5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="12">
         <v>0.83766470234400003</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -5094,11 +5439,15 @@
       <c r="K6" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="12">
         <v>0.745185017013</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -5130,11 +5479,15 @@
       <c r="K7" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="11">
         <v>0.91455116539299997</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -5166,11 +5519,15 @@
       <c r="K8" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="12">
         <v>0.83766470234400003</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -5199,11 +5556,15 @@
       <c r="K9" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="12">
         <v>0.745185017013</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -5229,14 +5590,18 @@
       <c r="J10" s="8">
         <v>0.96791792829400003</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="11">
         <v>0.948539697761</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="11">
         <v>0.94015559416399996</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -5257,7 +5622,7 @@
         <v>-1.5744860801656735</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -5278,7 +5643,7 @@
         <v>-1.0744860801656735</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -5299,7 +5664,7 @@
         <v>-0.57448608016567348</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:13">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -5320,7 +5685,7 @@
         <v>-7.4486080165673485E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:13">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -5341,7 +5706,7 @@
         <v>0.42551391983432652</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:13">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -5615,7 +5980,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B29" s="1">
@@ -5636,7 +6001,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B30" s="1">
@@ -5657,7 +6022,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="1">
@@ -5678,7 +6043,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="1">
@@ -5699,7 +6064,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B33" s="1">
@@ -5720,7 +6085,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="1">
@@ -5741,7 +6106,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="9" t="s">
         <v>105</v>
       </c>
       <c r="B35" s="1">
@@ -5796,10 +6161,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5811,10 +6176,12 @@
     <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
     <col min="6" max="8" width="10.83203125" style="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="10" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="15" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -5845,8 +6212,13 @@
       <c r="L1" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -5881,8 +6253,14 @@
       <c r="L2" s="7">
         <v>0.99975147672599995</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5914,8 +6292,14 @@
       <c r="L3" s="7">
         <v>0.998985958462</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="21"/>
+      <c r="O3" s="18"/>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -5950,8 +6334,14 @@
       <c r="L4" s="7">
         <v>0.998985958462</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="17"/>
+      <c r="O4" s="18"/>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -5986,8 +6376,14 @@
       <c r="L5" s="7">
         <v>0.99842407901300001</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="21"/>
+      <c r="O5" s="18"/>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -6019,8 +6415,14 @@
       <c r="L6" s="7">
         <v>0.99958226807499995</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="17"/>
+      <c r="O6" s="18"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -6055,8 +6457,14 @@
       <c r="L7" s="7">
         <v>0.99958226807499995</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N7" s="21"/>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -6082,17 +6490,23 @@
       <c r="I8" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="13">
         <v>0.93464181553400005</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="13">
         <v>0.93378804281500005</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8" s="13">
         <v>0.92704659702400005</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="17"/>
+      <c r="O8" s="18"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
@@ -6124,8 +6538,14 @@
       <c r="L9" s="7">
         <v>0.99985211948599995</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N9" s="21"/>
+      <c r="O9" s="18"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
@@ -6157,8 +6577,14 @@
       <c r="L10" s="7">
         <v>0.992050796131</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N10" s="17"/>
+      <c r="O10" s="18"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
@@ -6190,8 +6616,13 @@
       <c r="L11" s="7">
         <v>0.97489624470699998</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" t="b">
+        <v>1</v>
+      </c>
+      <c r="N11" s="21"/>
+      <c r="O11" s="18"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -6214,17 +6645,23 @@
       <c r="I12" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="14">
         <v>0.86739343944900005</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="14">
         <v>0.86748823433199995</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12" s="13">
         <v>0.89677821364300003</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="17"/>
+      <c r="O12" s="18"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -6247,17 +6684,23 @@
       <c r="I13" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.94860044146699996</v>
+      </c>
+      <c r="M13" s="15" t="b">
+        <f>FALSE</f>
         <v>0</v>
       </c>
-      <c r="K13" s="7">
-        <v>0</v>
-      </c>
-      <c r="L13" s="7">
-        <v>0.94860044146699996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="N13" s="21"/>
+      <c r="O13" s="18"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -6289,8 +6732,14 @@
       <c r="L14" s="7">
         <v>0.99994656745400001</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="21"/>
+      <c r="O14" s="18"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
@@ -6313,17 +6762,23 @@
       <c r="I15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="14">
         <v>0.74961493894800002</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="14">
         <v>0.76155258471999998</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="14">
         <v>0.80965286109400003</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="21"/>
+      <c r="O15" s="18"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
@@ -6346,17 +6801,23 @@
       <c r="I16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="13">
         <v>0.90626581554899999</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K16" s="13">
         <v>0.90586475468899996</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L16" s="13">
         <v>0.89677821364300003</v>
       </c>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="17"/>
+      <c r="O16" s="18"/>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
@@ -6388,8 +6849,14 @@
       <c r="L17" s="7">
         <v>0.98821727689100003</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="1" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="N17" s="21"/>
+      <c r="O17" s="18"/>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -6412,17 +6879,23 @@
       <c r="I18" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="13">
         <v>0.93464181553400005</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="13">
         <v>0.93378804281500005</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L18" s="13">
         <v>0.92704659702400005</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="17"/>
+      <c r="O18" s="18"/>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -6445,17 +6918,23 @@
       <c r="I19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="14">
         <v>0.81543857484399995</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="14">
         <v>0.81452997015999995</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="14">
         <v>0.814092605518</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="21"/>
+      <c r="O19" s="18"/>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -6478,17 +6957,23 @@
       <c r="I20" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="14">
         <v>0.86739343944900005</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="13">
         <v>0.90586475468899996</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L20" s="14">
         <v>0.85421887444800004</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="M20" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="21"/>
+      <c r="O20" s="18"/>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="s">
         <v>26</v>
       </c>
@@ -6520,8 +7005,14 @@
       <c r="L21" s="7">
         <v>0.999342116788</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="M21" s="15" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="21"/>
+      <c r="O21" s="18"/>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
@@ -6541,8 +7032,10 @@
         <f>F22-(5*LOG(E8, 10)-5)</f>
         <v>6.1340686579386308</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="N22" s="21"/>
+      <c r="O22" s="18"/>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -6562,8 +7055,10 @@
         <f>F23-(5*LOG(E8, 10)-5)</f>
         <v>6.6340686579386308</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="N23" s="21"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
@@ -6583,8 +7078,10 @@
         <f>F24-(5*LOG(E8, 10)-5)</f>
         <v>7.1340686579386308</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="N24" s="21"/>
+      <c r="O24" s="18"/>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -6604,8 +7101,10 @@
         <f>F25-(5*LOG(E8, 10)-5)</f>
         <v>7.6340686579386308</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="N25" s="21"/>
+      <c r="O25" s="18"/>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -6625,8 +7124,10 @@
         <f>F26-(5*LOG(E8, 10)-5)</f>
         <v>8.1340686579386308</v>
       </c>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="N26" s="17"/>
+      <c r="O26" s="18"/>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -6646,8 +7147,10 @@
         <f>F27-(5*LOG(E8, 10)-5)</f>
         <v>8.6340686579386308</v>
       </c>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="N27" s="21"/>
+      <c r="O27" s="18"/>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28" s="1" t="s">
         <v>33</v>
       </c>
@@ -6667,9 +7170,11 @@
         <f>F28-(5*LOG(E8, 10)-5)</f>
         <v>9.1340686579386308</v>
       </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" s="11" t="s">
+      <c r="N28" s="21"/>
+      <c r="O28" s="18"/>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="9" t="s">
         <v>99</v>
       </c>
       <c r="B29" s="1">
@@ -6688,9 +7193,11 @@
         <f>F29-(5*LOG(E8, 10)-5)</f>
         <v>9.6340686579386308</v>
       </c>
-    </row>
-    <row r="30" spans="1:12">
-      <c r="A30" s="11" t="s">
+      <c r="N29" s="21"/>
+      <c r="O29" s="18"/>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="9" t="s">
         <v>100</v>
       </c>
       <c r="B30" s="1">
@@ -6709,9 +7216,11 @@
         <f>F30-(5*LOG(E8, 10)-5)</f>
         <v>10.134068657938631</v>
       </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="11" t="s">
+      <c r="N30" s="21"/>
+      <c r="O30" s="18"/>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="9" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="1">
@@ -6730,9 +7239,11 @@
         <f>F31-(5*LOG(E8, 10)-5)</f>
         <v>10.634068657938631</v>
       </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" s="11" t="s">
+      <c r="N31" s="21"/>
+      <c r="O31" s="18"/>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="9" t="s">
         <v>102</v>
       </c>
       <c r="B32" s="1">
@@ -6751,9 +7262,11 @@
         <f>F32-(5*LOG(E8, 10)-5)</f>
         <v>11.134068657938631</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="11" t="s">
+      <c r="N32" s="17"/>
+      <c r="O32" s="18"/>
+    </row>
+    <row r="33" spans="1:15">
+      <c r="A33" s="9" t="s">
         <v>103</v>
       </c>
       <c r="B33" s="1">
@@ -6772,9 +7285,11 @@
         <f>F33-(5*LOG(E8, 10)-5)</f>
         <v>11.634068657938631</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="11" t="s">
+      <c r="N33" s="21"/>
+      <c r="O33" s="18"/>
+    </row>
+    <row r="34" spans="1:15">
+      <c r="A34" s="9" t="s">
         <v>104</v>
       </c>
       <c r="B34" s="1">
@@ -6793,11 +7308,15 @@
         <f>F34-(5*LOG(E8, 10)-5)</f>
         <v>12.134068657938631</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="11"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="N34" s="21"/>
+      <c r="O34" s="18"/>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="9"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="18"/>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -6813,11 +7332,87 @@
         <f>SUM(D2:D28)</f>
         <v>457069</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="N36" s="21"/>
+      <c r="O36" s="18"/>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="N37" s="21"/>
+      <c r="O37" s="18"/>
+    </row>
+    <row r="38" spans="1:15">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="18"/>
+    </row>
+    <row r="39" spans="1:15">
+      <c r="N39" s="21"/>
+      <c r="O39" s="18"/>
+    </row>
+    <row r="40" spans="1:15">
+      <c r="N40" s="21"/>
+      <c r="O40" s="18"/>
+    </row>
+    <row r="41" spans="1:15">
+      <c r="N41" s="21"/>
+      <c r="O41" s="18"/>
+    </row>
+    <row r="42" spans="1:15">
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+    </row>
+    <row r="43" spans="1:15">
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
+    </row>
+    <row r="44" spans="1:15">
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+    </row>
+    <row r="45" spans="1:15">
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+    </row>
+    <row r="46" spans="1:15">
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
+    </row>
+    <row r="47" spans="1:15">
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
+    </row>
+    <row r="48" spans="1:15">
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
+    </row>
+    <row r="49" spans="14:15">
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
+    </row>
+    <row r="50" spans="14:15">
+      <c r="N50" s="18"/>
+      <c r="O50" s="18"/>
+    </row>
+    <row r="51" spans="14:15">
+      <c r="N51" s="18"/>
+      <c r="O51" s="18"/>
+    </row>
+    <row r="52" spans="14:15">
+      <c r="N52" s="18"/>
+      <c r="O52" s="18"/>
+    </row>
+    <row r="53" spans="14:15">
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
+    </row>
+    <row r="54" spans="14:15">
+      <c r="N54" s="18"/>
+      <c r="O54" s="18"/>
+    </row>
+    <row r="55" spans="14:15">
+      <c r="N55" s="18"/>
+      <c r="O55" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>